<commit_message>
add puf code counts from documentation to xlsx recipes
</commit_message>
<xml_diff>
--- a/tmd/national_targets/data/target_recipes_v3.xlsx
+++ b/tmd/national_targets/data/target_recipes_v3.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="\\wsl.localhost\Ubuntu\home\donboyd5\Documents\mixed_projects\tax-microdata-benchmarking\tmd\national_targets\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7BDC0C8-FF84-4545-B320-F60D139607C4}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{796DEE73-B613-4549-A219-8AD69CE7EC0E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-109" yWindow="-109" windowWidth="46950" windowHeight="19060" activeTab="16" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
+    <workbookView xWindow="-109" yWindow="-109" windowWidth="46950" windowHeight="19060" firstSheet="4" activeTab="17" xr2:uid="{227C4D36-AC26-4B74-9955-EEE102DB4F9A}"/>
   </bookViews>
   <sheets>
     <sheet name="2026 notes" sheetId="35" r:id="rId1"/>
@@ -30,8 +30,9 @@
     <sheet name="stubmaps" sheetId="4" r:id="rId15"/>
     <sheet name="puf2015_vnames" sheetId="30" r:id="rId16"/>
     <sheet name="puf2015_wtdsums" sheetId="29" r:id="rId17"/>
-    <sheet name="puf2015_aggrecs" sheetId="23" r:id="rId18"/>
-    <sheet name="Sheet1" sheetId="31" r:id="rId19"/>
+    <sheet name="puf2015_codewtdcounts" sheetId="31" r:id="rId18"/>
+    <sheet name="puf2015_aggrecs" sheetId="23" r:id="rId19"/>
+    <sheet name="misc" sheetId="41" r:id="rId20"/>
   </sheets>
   <definedNames>
     <definedName name="ExternalData_1" localSheetId="12" hidden="1">puf_irs_map!#REF!</definedName>
@@ -71,7 +72,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3215" uniqueCount="1152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3252" uniqueCount="1172">
   <si>
     <t>table</t>
   </si>
@@ -3739,6 +3740,66 @@
   </si>
   <si>
     <t>form_location</t>
+  </si>
+  <si>
+    <t>code</t>
+  </si>
+  <si>
+    <t>2015 weighted counts</t>
+  </si>
+  <si>
+    <t>MARS</t>
+  </si>
+  <si>
+    <t>PUF 2015 documentation pp. 37-45</t>
+  </si>
+  <si>
+    <t>Marital (filing) status</t>
+  </si>
+  <si>
+    <t>code_description</t>
+  </si>
+  <si>
+    <t>Single</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Aggregated Return</t>
+  </si>
+  <si>
+    <t>Married filing a joint return or Widow(er) with dependent child (surviving spouse)</t>
+  </si>
+  <si>
+    <t>Married filing separately</t>
+  </si>
+  <si>
+    <t>Head of household</t>
+  </si>
+  <si>
+    <t>unknown-code5</t>
+  </si>
+  <si>
+    <t>unknown-code6</t>
+  </si>
+  <si>
+    <t>no-form</t>
+  </si>
+  <si>
+    <t>F1040_1</t>
+  </si>
+  <si>
+    <t>F1040_2</t>
+  </si>
+  <si>
+    <t>F1040_5</t>
+  </si>
+  <si>
+    <t>F1040_3</t>
+  </si>
+  <si>
+    <t>F1040_4</t>
+  </si>
+  <si>
+    <t>unknown</t>
   </si>
 </sst>
 </file>
@@ -4331,7 +4392,7 @@
     <xf numFmtId="40" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="204">
+  <cellXfs count="205">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -4866,6 +4927,7 @@
     <xf numFmtId="3" fontId="4" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="7">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -6573,6 +6635,143 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>940280</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>25879</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>8</xdr:col>
+      <xdr:colOff>65374</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>135916</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{01709B35-9369-AA65-64ED-23BB4CAD9AA6}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11464506" y="207034"/>
+          <a:ext cx="6095238" cy="3914286"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>810883</xdr:colOff>
+      <xdr:row>24</xdr:row>
+      <xdr:rowOff>103516</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>9</xdr:col>
+      <xdr:colOff>181543</xdr:colOff>
+      <xdr:row>38</xdr:row>
+      <xdr:rowOff>14969</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Picture 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{75434A66-469C-0825-7750-2A0A11F7EBD8}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11335109" y="4451229"/>
+          <a:ext cx="6961905" cy="2447619"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>1880559</xdr:colOff>
+      <xdr:row>20</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>669892</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>177512</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="4" name="Picture 3">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{C7229430-3DF4-5BEE-C8BC-75FF0143830C}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3"/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="2501661" y="3623094"/>
+          <a:ext cx="7933333" cy="3257143"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing8.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>434340</xdr:colOff>
       <xdr:row>2</xdr:row>
@@ -26322,11 +26521,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E3CF6E88-0F72-421E-9D3B-DEEEEEE10435}">
   <dimension ref="A1:E176"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane xSplit="1" ySplit="3" topLeftCell="B4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="B1" sqref="B1"/>
       <selection pane="bottomLeft" activeCell="A4" sqref="A4"/>
-      <selection pane="bottomRight" activeCell="E4" sqref="E4"/>
+      <selection pane="bottomRight" sqref="A1:E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
@@ -28885,11 +29084,259 @@
     <sortCondition ref="H4:H182"/>
   </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE26FC5C-AE67-4CBC-A48E-012CD3D25042}">
+  <dimension ref="A1:P33"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="29.75" customWidth="1"/>
+    <col min="4" max="4" width="66.75" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.125" customWidth="1"/>
+    <col min="6" max="6" width="12.875" customWidth="1"/>
+    <col min="7" max="7" width="12.125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="101" customWidth="1"/>
+    <col min="13" max="13" width="10.75" customWidth="1"/>
+    <col min="14" max="15" width="11.125" bestFit="1" customWidth="1"/>
+    <col min="16" max="17" width="10.75" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A1" s="1" t="s">
+        <v>1153</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A2" s="1" t="s">
+        <v>1155</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="1" t="s">
+        <v>1149</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1150</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>1152</v>
+      </c>
+      <c r="D3" s="1" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E3" s="1" t="s">
+        <v>1148</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>1147</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>1151</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B4" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C4">
+        <v>0</v>
+      </c>
+      <c r="D4" s="204" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E4">
+        <v>0</v>
+      </c>
+      <c r="F4" s="20">
+        <v>1233</v>
+      </c>
+      <c r="G4" t="s">
+        <v>1165</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C5">
+        <v>1</v>
+      </c>
+      <c r="D5" s="204" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E5" s="20">
+        <v>71086947</v>
+      </c>
+      <c r="F5" s="20">
+        <v>71257859</v>
+      </c>
+      <c r="G5" t="s">
+        <v>1166</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B6" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C6">
+        <v>2</v>
+      </c>
+      <c r="D6" s="204" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E6" s="20">
+        <v>54210327</v>
+      </c>
+      <c r="F6" s="20">
+        <v>54348677</v>
+      </c>
+      <c r="G6" t="s">
+        <v>1167</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B7" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C7">
+        <v>3</v>
+      </c>
+      <c r="D7" s="204" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E7" s="20">
+        <v>2947881</v>
+      </c>
+      <c r="F7" s="20">
+        <v>2919125</v>
+      </c>
+      <c r="G7" t="s">
+        <v>1169</v>
+      </c>
+      <c r="P7" s="20"/>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B8" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C8">
+        <v>4</v>
+      </c>
+      <c r="D8" s="204" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E8" s="20">
+        <v>22134303</v>
+      </c>
+      <c r="F8" s="20">
+        <v>22300953</v>
+      </c>
+      <c r="G8" t="s">
+        <v>1170</v>
+      </c>
+      <c r="P8" s="20"/>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B9" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C9">
+        <v>5</v>
+      </c>
+      <c r="D9" s="204" t="s">
+        <v>1163</v>
+      </c>
+      <c r="E9" s="20">
+        <v>84493</v>
+      </c>
+      <c r="F9" s="20">
+        <v>0</v>
+      </c>
+      <c r="G9" t="s">
+        <v>1168</v>
+      </c>
+      <c r="P9" s="20"/>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="204" t="s">
+        <v>1154</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1156</v>
+      </c>
+      <c r="C10">
+        <v>6</v>
+      </c>
+      <c r="D10" s="204" t="s">
+        <v>1164</v>
+      </c>
+      <c r="E10" s="20">
+        <v>29311</v>
+      </c>
+      <c r="F10" s="20">
+        <v>0</v>
+      </c>
+      <c r="G10" t="s">
+        <v>1171</v>
+      </c>
+      <c r="P10" s="20"/>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P11" s="20"/>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P12" s="20"/>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="P13" s="20"/>
+    </row>
+    <row r="33" spans="8:8" x14ac:dyDescent="0.25">
+      <c r="H33" s="2"/>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="M8:P26">
+    <sortCondition ref="M8:M26"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1E80C58B-BB4D-47DF-BCB6-D5A752D8EBB8}">
   <dimension ref="A1:G174"/>
   <sheetViews>
@@ -32877,118 +33324,6 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE26FC5C-AE67-4CBC-A48E-012CD3D25042}">
-  <dimension ref="B2:F13"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="U35" sqref="U35"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B2" s="1" t="s">
-        <v>465</v>
-      </c>
-      <c r="C2" s="1"/>
-      <c r="D2" s="1"/>
-      <c r="E2" s="1"/>
-      <c r="F2" s="1"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B3" t="s">
-        <v>111</v>
-      </c>
-      <c r="C3" t="s">
-        <v>112</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B4" t="s">
-        <v>298</v>
-      </c>
-      <c r="C4" t="s">
-        <v>114</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B5" t="s">
-        <v>300</v>
-      </c>
-      <c r="C5" t="s">
-        <v>116</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B6" t="s">
-        <v>117</v>
-      </c>
-      <c r="C6" t="s">
-        <v>118</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B7" t="s">
-        <v>166</v>
-      </c>
-      <c r="C7" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B8" t="s">
-        <v>137</v>
-      </c>
-      <c r="C8" t="s">
-        <v>138</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B9" t="s">
-        <v>151</v>
-      </c>
-      <c r="C9" t="s">
-        <v>152</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B10" t="s">
-        <v>180</v>
-      </c>
-      <c r="C10" t="s">
-        <v>181</v>
-      </c>
-    </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B11" t="s">
-        <v>393</v>
-      </c>
-      <c r="C11" t="s">
-        <v>132</v>
-      </c>
-    </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B12" t="s">
-        <v>120</v>
-      </c>
-      <c r="C12" t="s">
-        <v>121</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
-      <c r="B13" t="s">
-        <v>394</v>
-      </c>
-      <c r="C13" t="s">
-        <v>98</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{310844DF-F42E-4C0D-AB44-53E76321F1C8}">
   <dimension ref="B2:B5"/>
@@ -33029,6 +33364,118 @@
     <hyperlink ref="B4" r:id="rId3" xr:uid="{315DAA2F-1068-4EF8-92BF-542547A0B101}"/>
     <hyperlink ref="B5" r:id="rId4" xr:uid="{E0A86810-24E0-4F4B-AE3C-C3C3914057BD}"/>
   </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{27B606BA-77A3-46E6-BCB3-8461EA3CA18B}">
+  <dimension ref="B2:F13"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:K13"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.3" x14ac:dyDescent="0.25"/>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B2" s="1" t="s">
+        <v>465</v>
+      </c>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B3" t="s">
+        <v>111</v>
+      </c>
+      <c r="C3" t="s">
+        <v>112</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B4" t="s">
+        <v>298</v>
+      </c>
+      <c r="C4" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B5" t="s">
+        <v>300</v>
+      </c>
+      <c r="C5" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B6" t="s">
+        <v>117</v>
+      </c>
+      <c r="C6" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B7" t="s">
+        <v>166</v>
+      </c>
+      <c r="C7" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B8" t="s">
+        <v>137</v>
+      </c>
+      <c r="C8" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B9" t="s">
+        <v>151</v>
+      </c>
+      <c r="C9" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B10" t="s">
+        <v>180</v>
+      </c>
+      <c r="C10" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B11" t="s">
+        <v>393</v>
+      </c>
+      <c r="C11" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B12" t="s">
+        <v>120</v>
+      </c>
+      <c r="C12" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.25">
+      <c r="B13" t="s">
+        <v>394</v>
+      </c>
+      <c r="C13" t="s">
+        <v>98</v>
+      </c>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>